<commit_message>
[TEMP] Temporary save 20221126
</commit_message>
<xml_diff>
--- a/z0bug_odoo/z0bug_odoo/data/account_journal.xlsx
+++ b/z0bug_odoo/z0bug_odoo/data/account_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">portafolgio_sbf</t>
   </si>
   <si>
+    <t xml:space="preserve">effetti_allo_sconto</t>
+  </si>
+  <si>
     <t xml:space="preserve">limite_effetti_sbf</t>
   </si>
   <si>
@@ -149,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">z0bug.coa_180008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.coa_152220</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.bank14_journal</t>
@@ -294,7 +300,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -334,6 +340,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -378,7 +389,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,6 +422,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,17 +447,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="V6" activeCellId="0" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
@@ -461,7 +480,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="16.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,320 +550,332 @@
       <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>20</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="V4" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="0" t="n">
         <v>5000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>20</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S5" s="0" t="n">
         <v>80</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="V5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="W5" s="0" t="n">
         <v>2000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N6" s="7" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="R6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>100</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="V6" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="0" t="n">
         <v>2000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>25</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="6"/>
@@ -852,163 +883,163 @@
         <v>1</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I8" s="6" t="n">
         <v>7</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>5</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P9" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P10" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>20</v>
@@ -1017,154 +1048,154 @@
         <v>0</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>20</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L12" s="6" t="n">
         <v>0</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P12" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>15</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>16</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P14" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>

</xml_diff>